<commit_message>
fix: consertado problema que fazia não dar enter ao colar o número e exibir o pop-up errado.
</commit_message>
<xml_diff>
--- a/contravales.xlsx
+++ b/contravales.xlsx
@@ -368,7 +368,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A9"/>
+  <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -385,41 +385,26 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="n">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="n">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="n">
         <v>10</v>
       </c>
     </row>
@@ -434,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -471,6 +456,36 @@
       <c r="B3" t="inlineStr">
         <is>
           <t>2025-03-25 15:25:44</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>1</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>2025-03-25 15:58:44</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>2</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>2025-03-25 15:59:26</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>2025-03-25 15:59:57</t>
         </is>
       </c>
     </row>

</xml_diff>